<commit_message>
Revised implementation of link process partitioning and added DSI to air pollution controls
</commit_message>
<xml_diff>
--- a/data/Misc_Data/apcd_abbrev.xlsx
+++ b/data/Misc_Data/apcd_abbrev.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Box Sync\Research\05_Active_Research_Projects\Mass_Bal_CFPP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\trace_elem_mass_bal_repo\data\Misc_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1138,8 +1138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,7 +1409,7 @@
         <v>35</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
         <v>54</v>

</xml_diff>